<commit_message>
Worked on transform readme and lps/ras conversion
</commit_message>
<xml_diff>
--- a/amsaf/transform/transform_formatting.xlsx
+++ b/amsaf/transform/transform_formatting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Desktop/HART/amsaf/amsaf/transform_package/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Desktop/HART/amsaf/amsaf/Transform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEA1ED0-2EAD-014B-8D26-7600C4A717BF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0460BBB2-A30E-ED4C-87FD-AFABF62628F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>File In</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Verbose</t>
+  </si>
+  <si>
+    <t>RAS</t>
+  </si>
+  <si>
+    <t>Ox</t>
+  </si>
+  <si>
+    <t>Oy</t>
+  </si>
+  <si>
+    <t>Oz</t>
   </si>
 </sst>
 </file>
@@ -435,23 +447,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
       </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -502,6 +517,15 @@
       </c>
       <c r="Q2" t="s">
         <v>16</v>
+      </c>
+      <c r="R2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>